<commit_message>
modificacion Cita y agregar Medic.
</commit_message>
<xml_diff>
--- a/HOSPITAL_COVID.xlsx
+++ b/HOSPITAL_COVID.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B106264F-08FD-472E-8D2E-91DB16F83007}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -43,15 +42,6 @@
     <t>TELEFONO</t>
   </si>
   <si>
-    <t>PACIENTES</t>
-  </si>
-  <si>
-    <t>CITAS</t>
-  </si>
-  <si>
-    <t>COD PACIENTES</t>
-  </si>
-  <si>
     <t>TURNO</t>
   </si>
   <si>
@@ -64,9 +54,6 @@
     <t>COD_PACIENTES</t>
   </si>
   <si>
-    <t>COD_CITAS</t>
-  </si>
-  <si>
     <t>COD_DOCTOR</t>
   </si>
   <si>
@@ -173,12 +160,24 @@
   </si>
   <si>
     <t>Persona</t>
+  </si>
+  <si>
+    <t>CITA</t>
+  </si>
+  <si>
+    <t>PACIENTE</t>
+  </si>
+  <si>
+    <t>COD_PACIENTE</t>
+  </si>
+  <si>
+    <t>COD PACIENTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,11 +560,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,31 +594,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="G2" s="4">
         <v>3</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="J2" s="4">
         <v>4</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="M2" s="4">
         <v>5</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -627,17 +626,17 @@
         <v>0</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -647,8 +646,8 @@
       <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
+      <c r="H4" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>1</v>
@@ -664,8 +663,8 @@
       <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>49</v>
+      <c r="H5" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>2</v>
@@ -682,10 +681,10 @@
         <v>2</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>6</v>
@@ -696,18 +695,18 @@
         <v>4</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>18</v>
+      <c r="H8" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>6</v>
@@ -718,7 +717,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -731,90 +730,90 @@
         <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>7</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G12">
         <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J12">
         <v>9</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="M12">
         <v>10</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>1</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>5</v>
@@ -822,21 +821,21 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>6</v>
@@ -844,7 +843,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E19" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="18.75" x14ac:dyDescent="0.4">
@@ -852,30 +851,30 @@
         <v>11</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <v>12</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G22" s="13">
         <v>13</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -883,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>1</v>
@@ -891,36 +890,36 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H27" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H28" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H29" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrega 3 clases:HistoClin, RecMed, TipPrueba
</commit_message>
<xml_diff>
--- a/HOSPITAL_COVID.xlsx
+++ b/HOSPITAL_COVID.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7206CD0E-6652-4B42-8F48-51503117F51F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>DNI</t>
   </si>
@@ -148,9 +149,6 @@
   </si>
   <si>
     <t>COD_VACUNA</t>
-  </si>
-  <si>
-    <t>CITA DE CONTROL</t>
   </si>
   <si>
     <t xml:space="preserve">PAIS DE PROCEDENCIA </t>
@@ -177,7 +175,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +220,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +236,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -288,17 +292,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,11 +581,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,31 +614,31 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>50</v>
+      <c r="B2" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>46</v>
+      <c r="H2" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="J2" s="3">
         <v>4</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="3">
         <v>5</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -644,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="7" t="s">
@@ -665,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>1</v>
@@ -724,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>6</v>
@@ -735,13 +738,16 @@
         <v>5</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
@@ -753,7 +759,7 @@
       <c r="D12">
         <v>7</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G12">
@@ -765,7 +771,7 @@
       <c r="J12">
         <v>9</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="14" t="s">
         <v>24</v>
       </c>
       <c r="M12">
@@ -868,30 +874,22 @@
       <c r="A22">
         <v>11</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D22">
         <v>12</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="11">
-        <v>13</v>
-      </c>
-      <c r="H22" s="16" t="s">
+      <c r="E22" s="14" t="s">
         <v>41</v>
       </c>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -900,9 +898,6 @@
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -910,10 +905,7 @@
       <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -921,23 +913,23 @@
       <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H29" s="5" t="s">
-        <v>44</v>
+      <c r="E29" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>